<commit_message>
Update product import template
</commit_message>
<xml_diff>
--- a/public/files/templates/product.xlsx
+++ b/public/files/templates/product.xlsx
@@ -20,11 +20,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t xml:space="preserve">Template Product</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No</t>
+  </si>
   <si>
     <t xml:space="preserve">Code</t>
   </si>
   <si>
+    <t xml:space="preserve">Product Category Code</t>
+  </si>
+  <si>
     <t xml:space="preserve">Name</t>
   </si>
   <si>
@@ -34,7 +43,10 @@
     <t xml:space="preserve">Price</t>
   </si>
   <si>
-    <t xml:space="preserve">Initial Stock</t>
+    <t xml:space="preserve">Part Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brand</t>
   </si>
   <si>
     <t xml:space="preserve">Stock</t>
@@ -113,9 +125,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -139,46 +155,70 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
+      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="6.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="20"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="C2" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:I1"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>